<commit_message>
fixing performance table error
</commit_message>
<xml_diff>
--- a/prod_manage_QA/mobile_manual_testing/system_testing/TST_SISTEMA_ProdManage_16-09-2024.xlsx
+++ b/prod_manage_QA/mobile_manual_testing/system_testing/TST_SISTEMA_ProdManage_16-09-2024.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Sumário" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="89">
   <si>
     <t>Projeto</t>
   </si>
@@ -414,12 +414,6 @@
     <t>1- O botão "Cronometrar" deve ficar indisponível, apenas aparecendo o botão de "Salvar Rendimento".</t>
   </si>
   <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>Dados são apagados sempre que saio e volto para a página.</t>
-  </si>
-  <si>
     <t>1- Entrar na tela "Rendimento";
 2- Preencher as colunas com valores maiores e menores que a meta "70%".</t>
   </si>
@@ -437,6 +431,9 @@
   </si>
   <si>
     <t>Novos cenários adicionados.</t>
+  </si>
+  <si>
+    <t>Arrumando erro de não salvar dados da tabela.</t>
   </si>
 </sst>
 </file>
@@ -803,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -883,9 +880,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1098,7 +1092,9 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1125,10 +1121,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1150,6 +1146,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1490,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,11 +1511,11 @@
       <c r="B2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="35"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -1566,7 +1563,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1576,9 +1573,15 @@
       <c r="B6" s="27">
         <v>45551</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="28"/>
+      <c r="E6" s="24">
+        <v>45555</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -1587,9 +1590,9 @@
       <c r="B7" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1605,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1495"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,7 +1985,7 @@
         <v>77</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>79</v>
@@ -2023,20 +2026,18 @@
         <v>66</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="F19" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>84</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
@@ -22815,11 +22816,11 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -22839,11 +22840,11 @@
       </c>
       <c r="B4" s="10">
         <f>COUNTIF(Cenários!F:F,"OK")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="13">
         <f>B4/B3</f>
-        <v>0.94736842105263153</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -22852,11 +22853,11 @@
       </c>
       <c r="B5" s="10">
         <f>COUNTIF(Cenários!F:F,"NOK")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="13">
         <f>B5/B3</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>